<commit_message>
Updates original input PE table
</commit_message>
<xml_diff>
--- a/DataExtracts/Poverty_and_Equity.xlsx
+++ b/DataExtracts/Poverty_and_Equity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katedannemiller/Documents/DA401/CovidPrep/DataExtracts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B988C96-6C96-3343-A72D-6552BA0AEB13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0517476A-F8EE-494F-BF85-301774325A1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="1060" windowWidth="24560" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4240" yWindow="1060" windowWidth="24560" windowHeight="14440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DK" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="252">
   <si>
     <t>Poverty headcount ratio at $1.90 a day, with secondary education (2011 PPP) (% of population age 16+ with secondary education)</t>
   </si>
@@ -1180,7 +1180,7 @@
   <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A43" sqref="A43:A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1460,20 +1460,16 @@
       <c r="C42" s="2"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-      <c r="C43" s="2"/>
+      <c r="B43" s="2"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="C44" s="2"/>
+      <c r="B44" s="2"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="B45" s="2"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="C46" s="2"/>
+      <c r="B46" s="2"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
@@ -1645,7 +1641,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A43" sqref="A43:A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1899,26 +1895,6 @@
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>155</v>
-      </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>

</xml_diff>